<commit_message>
ΚΑΛΟ UPDATE VOL 2
</commit_message>
<xml_diff>
--- a/data/tony/excel/802576637_2025_invoices.xlsx
+++ b/data/tony/excel/802576637_2025_invoices.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,106 +498,56 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>400011576793993</t>
+          <t>400011615024455</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>998345385</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
+          <t>800916954</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ΑΦΟΙ ΛΑΓΟΥ ΧΡΩΜΑΤΑ ΙΚΕ</t>
+        </is>
+      </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ΑΛΠ</t>
+          <t>TΔA</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>130739</t>
+          <t>60984</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>31/10/2025</t>
+          <t>11/11/2025</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>ΑΠΟΔΕΙΞΗ</t>
+          <t>Τιμολόγιο Πώλησης</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2,60</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr"/>
+          <t>104,99</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>23,91</t>
+        </is>
+      </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2,60</t>
+          <t>128,90</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
-        <is>
-          <t>130739</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>400011615024455</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>800916954</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>ΑΦΟΙ ΛΑΓΟΥ ΧΡΩΜΑΤΑ ΙΚΕ</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>TΔA</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>60984</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>11/11/2025</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Τιμολόγιο Πώλησης</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>104,99</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>23,91</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>128,90</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
         <is>
           <t>60984</t>
         </is>

</xml_diff>